<commit_message>
got lc3 to work
....now we just need to make some cool figs
</commit_message>
<xml_diff>
--- a/climate/5min_1yrRI_storm.xlsx
+++ b/climate/5min_1yrRI_storm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\MultiGrain\climate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259AE354-3347-4E01-BB5E-68CA3D988D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477FB41E-BA79-4BC1-99B6-4C63BB172B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,7 +361,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,7 +382,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>99.37</v>
+        <v>445.00799999999998</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -390,7 +390,7 @@
         <v>60</v>
       </c>
       <c r="B3">
-        <v>99.37</v>
+        <v>445.00799999999998</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -398,7 +398,7 @@
         <v>120</v>
       </c>
       <c r="B4">
-        <v>99.37</v>
+        <v>445.00799999999998</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -406,7 +406,7 @@
         <v>180</v>
       </c>
       <c r="B5">
-        <v>99.37</v>
+        <v>445.00799999999998</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -414,7 +414,7 @@
         <v>240</v>
       </c>
       <c r="B6">
-        <v>99.37</v>
+        <v>445.00799999999998</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -422,7 +422,7 @@
         <v>300</v>
       </c>
       <c r="B7">
-        <v>99.37</v>
+        <v>445.00799999999998</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -443,5 +443,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>